<commit_message>
automation for ASGS implemented
</commit_message>
<xml_diff>
--- a/Classifications/LOCATION_ASGS/Download/MB_Data_Source.xlsx
+++ b/Classifications/LOCATION_ASGS/Download/MB_Data_Source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f6894d554b36768a/Documents/GIthub/abs/Classifications/LOCATION_ASGS/Download/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7B63B2A-085D-4320-994A-660EE5478F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{F7B63B2A-085D-4320-994A-660EE5478F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9512ED7B-C289-4097-A0A0-93E772B85FE1}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{AD34235C-85A6-4279-A34D-0567055999CA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>url</t>
   </si>
@@ -96,6 +96,18 @@
   </si>
   <si>
     <t>1270055001_mb_2016_ot_csv.zip</t>
+  </si>
+  <si>
+    <t>https://www.abs.gov.au/ausstats/subscriber.nsf/log?openagent&amp;1270055004_sa1_ucl_sosr_sos_2016_aust_csv.zip&amp;1270.0.55.004&amp;Data%20Cubes&amp;EE5F4698A91AD2F8CA2581B1000E09B0&amp;0&amp;July%202016&amp;09.10.2017&amp;Latest</t>
+  </si>
+  <si>
+    <t>https://www.abs.gov.au/ausstats/subscriber.nsf/log?openagent&amp;1270055004_sa2_sua_2016_aust_csv.zip&amp;1270.0.55.004&amp;Data%20Cubes&amp;D6E51168BD6DC248CA2581B1000E0A48&amp;0&amp;July%202016&amp;09.10.2017&amp;Latest</t>
+  </si>
+  <si>
+    <t>1270055004_sa2_sua_2016_aust_csv.zip</t>
+  </si>
+  <si>
+    <t>1270055004_sa1_ucl_sosr_sos_2016_aust_csv.zip</t>
   </si>
 </sst>
 </file>
@@ -478,16 +490,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1EDEBC-02D2-4B9D-9452-BBEE072D5D4E}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="187.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="201.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -568,6 +580,22 @@
       </c>
       <c r="B10" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -580,6 +608,8 @@
     <hyperlink ref="A8" r:id="rId6" xr:uid="{DA4AF5D5-910D-4DE4-86C4-C1030CE7CE02}"/>
     <hyperlink ref="A9" r:id="rId7" xr:uid="{EB7727A4-FEC6-4E3E-9B24-95B62CF8C5DC}"/>
     <hyperlink ref="A10" r:id="rId8" xr:uid="{F13C94F4-BE22-4C98-BFFD-03EBC775BBD2}"/>
+    <hyperlink ref="A12" r:id="rId9" xr:uid="{1EC75B8E-11AF-497E-8BFA-5D799DC2787E}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{0F730FC3-C9B3-4388-9993-AB635AE84442}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>